<commit_message>
info pode ser util, ver o 31, falta concluir os mini graficos da Column e Row
</commit_message>
<xml_diff>
--- a/proj2AAD/incOrderCuda.xlsx
+++ b/proj2AAD/incOrderCuda.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victm\OneDrive\Ambiente de Trabalho\UNI\AAD\projetoAAD\proj2AAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\repol\Documents\GitHub\projetoAAD\proj2AAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E9CD61-C193-4DDB-B93E-DDFC2AB050D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98F6C7D-9ACC-43E4-B3A2-454DDC661303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="4500" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Colunas" sheetId="1" r:id="rId1"/>
     <sheet name="Linhas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -603,69 +603,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="108">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000E+00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1731,6 +1668,69 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1759,42 +1759,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Curva</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> da coluna</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1826,7 +1790,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1862,7 +1826,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Colunas!$O$4:$O$14</c:f>
+              <c:f>Colunas!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1977,7 +1941,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Colunas!$O$4:$O$14</c:f>
+              <c:f>Colunas!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2085,23 +2049,10 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="high"/>
+        <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2131,7 +2082,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="388859928"/>
@@ -2151,35 +2102,8 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="5000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
         <c:numFmt formatCode="0.0000E+00" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -2205,7 +2129,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="388859272"/>
@@ -2246,7 +2170,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2294,7 +2218,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2382,7 +2306,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2418,7 +2342,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Colunas!$O$4:$O$14</c:f>
+              <c:f>Colunas!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2533,7 +2457,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Colunas!$O$4:$O$14</c:f>
+              <c:f>Colunas!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2577,7 +2501,7 @@
             <c:numRef>
               <c:f>Colunas!$M$36:$M$46</c:f>
               <c:numCache>
-                <c:formatCode>0\.0000E+00</c:formatCode>
+                <c:formatCode>0.0000E+00</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>0.12426</c:v>
@@ -2687,7 +2611,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="388859928"/>
@@ -2748,7 +2672,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="388859272"/>
@@ -2789,7 +2713,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2837,7 +2761,1210 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Curva da linha</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Media Linha a cima</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Colunas!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Colunas!$K$49:$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.1566E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.5888000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.7808000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12418</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D580-4975-92B6-832592403E14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Media Linha a baixo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Colunas!$K$56:$K$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.1566E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2310000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11838</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13317999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14138000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47497999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D580-4975-92B6-832592403E14}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="388859272"/>
+        <c:axId val="388859928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="388859272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="high"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388859928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="388859928"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5"/>
+          <c:min val="1.0000000000000002E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0.0000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388859272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Colunas!$K$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Media</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Colunas!$E$17:$E$22</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>&lt;&lt;&lt;(32,1,1),(32,1,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;&lt;&lt;(32,2,1), (16,1,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;&lt;&lt;(32,4,1), (8,1,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;&lt;&lt;(32,8,1), (4,1,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;&lt;&lt;(32,16,1), (2,1,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;&lt;&lt;(32,32,1), (1,1,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Colunas!$K$17:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>0\.0000E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.14287999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15255999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15336</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15615999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20762</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.23494000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7307-4FC2-B4F6-3E8E5030E923}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="388859272"/>
+        <c:axId val="388859928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="388859272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388859928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="388859928"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0\.0000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388859272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Colunas!$K$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Media</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Colunas!$E$25:$E$30</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>&lt;&lt;&lt;(32,1,1),(32,1,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>&lt;&lt;&lt;(16,1,1), (32,2,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>&lt;&lt;&lt;(8,1,1), (32,4,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>&lt;&lt;&lt;(4,1,1), (32,8,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>&lt;&lt;&lt;(2,1,1), (32,16,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>&lt;&lt;&lt;(1,1,1), (32,32,1)&gt;&gt;&gt;</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Colunas!$K$25:$K$30</c:f>
+              <c:numCache>
+                <c:formatCode>0\.0000E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.14287999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14687999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.15201999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15514</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16838000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-04DE-4865-9C98-48837BC7ADC1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="388859272"/>
+        <c:axId val="388859928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="388859272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388859928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="388859928"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0\.0000E+00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="388859272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2928,6 +4055,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -3920,20 +5167,1508 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>566696</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>18891</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>132830</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>24605</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>174811</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>72358</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>294410</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>3809</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3960,16 +6695,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>576943</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>174171</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>77661</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38831</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>185058</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>299356</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>292505</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>102006</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3996,31 +6731,145 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>115340</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>51954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>17318</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F082276-C646-428A-A1F5-1DBF78137529}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>134736</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>155863</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>242455</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>34637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10BBD8EE-5382-4352-ADAB-A6B93B04B881}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>115339</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>58068</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90C96BF3-E49F-4E35-8884-EECA657D7926}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C74EBD76-2F64-4221-A5A3-4D464FC5AECB}" name="Tabela4" displayName="Tabela4" ref="B3:M14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C74EBD76-2F64-4221-A5A3-4D464FC5AECB}" name="Tabela4" displayName="Tabela4" ref="B3:M14" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="B3:M14" xr:uid="{C74EBD76-2F64-4221-A5A3-4D464FC5AECB}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A4FB5ABB-A987-4CA2-B11A-C8B2C50322A2}" name="gridDimX" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{3876FD4E-04AA-4F68-B1F5-7CB98751491F}" name="blockDimX" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{6B3C28D5-159B-4BAA-8B6A-7B2D5B99FFF9}" name="Cuda Kernel" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{FA98D974-7A36-4234-AAFA-1D60412A6199}" name="1º " dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{D6494B06-A91B-4055-920C-2BA070345A57}" name="2º" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{3E319409-4F31-446E-84F7-DDC5D5D0B016}" name="3º" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{2D2FC63D-5D57-4D44-9590-D45C0573E388}" name="4º" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{B5013285-D899-4EE0-B9C1-FB2FA691672C}" name="5º" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{0B471454-963B-4030-90BE-C33AC2C7C5D8}" name="Media" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{A4FB5ABB-A987-4CA2-B11A-C8B2C50322A2}" name="gridDimX" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{3876FD4E-04AA-4F68-B1F5-7CB98751491F}" name="blockDimX" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{6B3C28D5-159B-4BAA-8B6A-7B2D5B99FFF9}" name="Cuda Kernel" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{FA98D974-7A36-4234-AAFA-1D60412A6199}" name="1º " dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{D6494B06-A91B-4055-920C-2BA070345A57}" name="2º" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{3E319409-4F31-446E-84F7-DDC5D5D0B016}" name="3º" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{2D2FC63D-5D57-4D44-9590-D45C0573E388}" name="4º" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{B5013285-D899-4EE0-B9C1-FB2FA691672C}" name="5º" dataDxfId="98"/>
+    <tableColumn id="9" xr3:uid="{0B471454-963B-4030-90BE-C33AC2C7C5D8}" name="Media" dataDxfId="97">
       <calculatedColumnFormula>AVERAGE(E4:I4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{D7FE7045-EE1F-4D54-B2F4-26B2C0CF0E29}" name="Desvio Padrao" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{D7FE7045-EE1F-4D54-B2F4-26B2C0CF0E29}" name="Desvio Padrao" dataDxfId="96">
       <calculatedColumnFormula>STDEV(E4:I4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{26791600-D0E6-4339-BB36-441C5D26FD18}" name="Coef" dataDxfId="1">
+    <tableColumn id="11" xr3:uid="{26791600-D0E6-4339-BB36-441C5D26FD18}" name="Coef" dataDxfId="95">
       <calculatedColumnFormula>Tabela4[[#This Row],[Media]]/Tabela4[[#This Row],[Desvio Padrao]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{824E85EC-7E92-4CF0-BB44-5B38407A765D}" name="Teorica" dataDxfId="0">
+    <tableColumn id="12" xr3:uid="{824E85EC-7E92-4CF0-BB44-5B38407A765D}" name="Teorica" dataDxfId="94">
       <calculatedColumnFormula>AVERAGE(H4:L4)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4029,21 +6878,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DC14E98F-30DC-4A1B-8D50-0724132F1414}" name="Tabela5" displayName="Tabela5" ref="C97:L108" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DC14E98F-30DC-4A1B-8D50-0724132F1414}" name="Tabela5" displayName="Tabela5" ref="C97:L108" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="C97:L108" xr:uid="{DC14E98F-30DC-4A1B-8D50-0724132F1414}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{38E84C7C-5593-47A0-B9FE-97ED10C29DCA}" name="gridDimY" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{940C2EDA-81D0-4130-BEF9-A829F5C414D2}" name="blockDimY" dataDxfId="104"/>
-    <tableColumn id="3" xr3:uid="{874CBB69-F465-41D5-B91B-D1C7B9BA9206}" name="Cuda Kernel" dataDxfId="103"/>
-    <tableColumn id="4" xr3:uid="{74A2729D-E2F0-4244-A880-E693541D4AF9}" name="1º " dataDxfId="102"/>
-    <tableColumn id="5" xr3:uid="{6A3ED035-4D76-47E0-9DC8-66DB9C6123C6}" name="2º" dataDxfId="101"/>
-    <tableColumn id="6" xr3:uid="{13CEAE3D-1169-4B60-AD8C-648131971D32}" name="3º" dataDxfId="100"/>
-    <tableColumn id="7" xr3:uid="{4692D76D-DC60-4F85-BAC0-9C812CE8951A}" name="4º" dataDxfId="99"/>
-    <tableColumn id="8" xr3:uid="{DAC5E63F-DC48-4399-8459-18213A8259B4}" name="5º" dataDxfId="98"/>
-    <tableColumn id="9" xr3:uid="{705BFBC0-7739-4CB3-BC01-4A19BF93EDF7}" name="Media" dataDxfId="97">
+    <tableColumn id="1" xr3:uid="{38E84C7C-5593-47A0-B9FE-97ED10C29DCA}" name="gridDimY" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{940C2EDA-81D0-4130-BEF9-A829F5C414D2}" name="blockDimY" dataDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{874CBB69-F465-41D5-B91B-D1C7B9BA9206}" name="Cuda Kernel" dataDxfId="89"/>
+    <tableColumn id="4" xr3:uid="{74A2729D-E2F0-4244-A880-E693541D4AF9}" name="1º " dataDxfId="88"/>
+    <tableColumn id="5" xr3:uid="{6A3ED035-4D76-47E0-9DC8-66DB9C6123C6}" name="2º" dataDxfId="87"/>
+    <tableColumn id="6" xr3:uid="{13CEAE3D-1169-4B60-AD8C-648131971D32}" name="3º" dataDxfId="86"/>
+    <tableColumn id="7" xr3:uid="{4692D76D-DC60-4F85-BAC0-9C812CE8951A}" name="4º" dataDxfId="85"/>
+    <tableColumn id="8" xr3:uid="{DAC5E63F-DC48-4399-8459-18213A8259B4}" name="5º" dataDxfId="84"/>
+    <tableColumn id="9" xr3:uid="{705BFBC0-7739-4CB3-BC01-4A19BF93EDF7}" name="Media" dataDxfId="83">
       <calculatedColumnFormula>AVERAGE(F98:J98)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0A879FFD-5E80-429D-A497-5245B8D8C9E9}" name="Desvio Padrao" dataDxfId="96">
+    <tableColumn id="10" xr3:uid="{0A879FFD-5E80-429D-A497-5245B8D8C9E9}" name="Desvio Padrao" dataDxfId="82">
       <calculatedColumnFormula>STDEV(F98:J98)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4052,25 +6901,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74ED20E1-E8E4-4B3D-A14C-5E1F6953877E}" name="Tabela1" displayName="Tabela1" ref="B16:M22" totalsRowShown="0" headerRowDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{74ED20E1-E8E4-4B3D-A14C-5E1F6953877E}" name="Tabela1" displayName="Tabela1" ref="B16:M22" totalsRowShown="0" headerRowDxfId="81">
   <autoFilter ref="B16:M22" xr:uid="{74ED20E1-E8E4-4B3D-A14C-5E1F6953877E}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{52E6AFB4-5DF1-47BD-9568-3B299002770C}" name="gridDimX" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{B60B7410-FADE-4250-905C-FD042699A4D9}" name="gridDimY" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{A85E00EB-F6EF-45A3-B443-FFFF0BEA471D}" name="blockDimX2" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{DBFB7FBC-E871-4AC4-AC2A-D469262040A1}" name="Cuda Kernel" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{2172D3BF-AE72-473C-9641-FDB4A1680270}" name="1º " dataDxfId="90"/>
-    <tableColumn id="6" xr3:uid="{2B701978-FCA1-4C82-9D9B-DE022FB4A4FF}" name="2º" dataDxfId="89"/>
-    <tableColumn id="7" xr3:uid="{6DA80BDC-4444-40AB-A685-82DAC3912666}" name="3º" dataDxfId="88"/>
-    <tableColumn id="8" xr3:uid="{038A9259-EC36-4014-A0B2-0F26E0672A32}" name="4º" dataDxfId="87"/>
-    <tableColumn id="9" xr3:uid="{C2163FB8-415E-49C3-8BA1-0EC46171FBF3}" name="5º" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{52E6AFB4-5DF1-47BD-9568-3B299002770C}" name="gridDimX" dataDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{B60B7410-FADE-4250-905C-FD042699A4D9}" name="gridDimY" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{A85E00EB-F6EF-45A3-B443-FFFF0BEA471D}" name="blockDimX2" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{DBFB7FBC-E871-4AC4-AC2A-D469262040A1}" name="Cuda Kernel" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{2172D3BF-AE72-473C-9641-FDB4A1680270}" name="1º " dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{2B701978-FCA1-4C82-9D9B-DE022FB4A4FF}" name="2º" dataDxfId="75"/>
+    <tableColumn id="7" xr3:uid="{6DA80BDC-4444-40AB-A685-82DAC3912666}" name="3º" dataDxfId="74"/>
+    <tableColumn id="8" xr3:uid="{038A9259-EC36-4014-A0B2-0F26E0672A32}" name="4º" dataDxfId="73"/>
+    <tableColumn id="9" xr3:uid="{C2163FB8-415E-49C3-8BA1-0EC46171FBF3}" name="5º" dataDxfId="72"/>
     <tableColumn id="10" xr3:uid="{DE062FC4-CCA3-4157-AD17-BD34AAB63B56}" name="Media">
       <calculatedColumnFormula>AVERAGE(F17:J17)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{98658D6C-7C17-4CB3-B7A4-9A219E991DF4}" name="Desvio Padrao">
       <calculatedColumnFormula>STDEV(F17:J17)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{48060F8B-9519-4243-A151-D5212C9BDD42}" name="Coef" dataDxfId="85">
+    <tableColumn id="12" xr3:uid="{48060F8B-9519-4243-A151-D5212C9BDD42}" name="Coef" dataDxfId="71">
       <calculatedColumnFormula>Tabela1[[#This Row],[Media]]/Tabela1[[#This Row],[Desvio Padrao]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4079,25 +6928,25 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2F53E0B9-0593-4C1C-B2A0-1837C1B5A266}" name="Tabela13" displayName="Tabela13" ref="B24:M30" totalsRowShown="0" headerRowDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2F53E0B9-0593-4C1C-B2A0-1837C1B5A266}" name="Tabela13" displayName="Tabela13" ref="B24:M30" totalsRowShown="0" headerRowDxfId="70">
   <autoFilter ref="B24:M30" xr:uid="{2F53E0B9-0593-4C1C-B2A0-1837C1B5A266}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{D314A26A-776E-45AB-B97C-7B4CCD10C6FF}" name="gridDimX" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{327AC6DC-C1F5-48BB-87F3-B8A02C7E2686}" name="blockDimY" dataDxfId="82"/>
-    <tableColumn id="3" xr3:uid="{021914CB-903B-46D1-8C0C-D57FF48C53D2}" name="blockDimX" dataDxfId="81"/>
-    <tableColumn id="4" xr3:uid="{22CF2BAA-EAE0-40FD-924F-104AA7269971}" name="Cuda Kernel" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{559B6EDE-E5F1-4467-9BB6-56E53367D8CD}" name="1º " dataDxfId="79"/>
-    <tableColumn id="6" xr3:uid="{5A68E55B-82E9-48A4-88E3-1AEE8F151CAC}" name="2º" dataDxfId="78"/>
-    <tableColumn id="7" xr3:uid="{BD5633D2-A4BE-46EB-92DC-4B5C8E36B953}" name="3º" dataDxfId="77"/>
-    <tableColumn id="8" xr3:uid="{716DB042-307B-4AC2-83FC-424454FD69CD}" name="4º" dataDxfId="76"/>
-    <tableColumn id="9" xr3:uid="{71CE32D6-C326-404D-9201-6899B768CA45}" name="5º" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{D314A26A-776E-45AB-B97C-7B4CCD10C6FF}" name="gridDimX" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{327AC6DC-C1F5-48BB-87F3-B8A02C7E2686}" name="blockDimY" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{021914CB-903B-46D1-8C0C-D57FF48C53D2}" name="blockDimX" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{22CF2BAA-EAE0-40FD-924F-104AA7269971}" name="Cuda Kernel" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{559B6EDE-E5F1-4467-9BB6-56E53367D8CD}" name="1º " dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{5A68E55B-82E9-48A4-88E3-1AEE8F151CAC}" name="2º" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{BD5633D2-A4BE-46EB-92DC-4B5C8E36B953}" name="3º" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{716DB042-307B-4AC2-83FC-424454FD69CD}" name="4º" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{71CE32D6-C326-404D-9201-6899B768CA45}" name="5º" dataDxfId="61"/>
     <tableColumn id="10" xr3:uid="{0DBD358B-300C-4033-AA0E-A3DCB21D8500}" name="Media">
       <calculatedColumnFormula>AVERAGE(F25:J25)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{E3982694-B84F-468F-8E7A-C71D6B7CBE65}" name="Desvio Padrao">
       <calculatedColumnFormula>STDEV(F25:J25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{45C0EDE9-14CC-4827-833A-038644AD1D14}" name="Coef" dataDxfId="74">
+    <tableColumn id="12" xr3:uid="{45C0EDE9-14CC-4827-833A-038644AD1D14}" name="Coef" dataDxfId="60">
       <calculatedColumnFormula>Tabela1[[#This Row],[Media]]/Tabela1[[#This Row],[Desvio Padrao]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4106,27 +6955,27 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03C0836E-B1EE-4D75-99BB-3F36F1FF92FB}" name="Tabela44" displayName="Tabela44" ref="B35:M46" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03C0836E-B1EE-4D75-99BB-3F36F1FF92FB}" name="Tabela44" displayName="Tabela44" ref="B35:M46" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="B35:M46" xr:uid="{03C0836E-B1EE-4D75-99BB-3F36F1FF92FB}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{388DE001-89BA-417E-B7EF-7A0BECF6E67D}" name="gridDimX" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{D648D2C6-DD68-4C3F-9213-97BEDE7270EC}" name="blockDimX2" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{65C6110F-6C96-4499-A0D3-52D5B3BAC0A4}" name="Cuda Kernel" dataDxfId="69"/>
-    <tableColumn id="4" xr3:uid="{891A908C-D473-4397-A84B-774BF1B3D63F}" name="1º " dataDxfId="68"/>
-    <tableColumn id="5" xr3:uid="{0A8CA49E-ADD6-4811-BA9A-4DF6C1DE7825}" name="2º" dataDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{B74082CB-C724-4E93-A0D3-B6DCA9273989}" name="3º" dataDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{54F448C8-ECFC-473A-BEE4-96E23DAC0F3B}" name="4º" dataDxfId="65"/>
-    <tableColumn id="8" xr3:uid="{850D29A6-7DF0-4D99-8BA8-FDAD97B3836A}" name="5º" dataDxfId="64"/>
-    <tableColumn id="9" xr3:uid="{D9466A68-3B98-471D-BCE1-46483F4DD230}" name="Media" dataDxfId="63">
+    <tableColumn id="1" xr3:uid="{388DE001-89BA-417E-B7EF-7A0BECF6E67D}" name="gridDimX" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{D648D2C6-DD68-4C3F-9213-97BEDE7270EC}" name="blockDimX2" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{65C6110F-6C96-4499-A0D3-52D5B3BAC0A4}" name="Cuda Kernel" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{891A908C-D473-4397-A84B-774BF1B3D63F}" name="1º " dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{0A8CA49E-ADD6-4811-BA9A-4DF6C1DE7825}" name="2º" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{B74082CB-C724-4E93-A0D3-B6DCA9273989}" name="3º" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{54F448C8-ECFC-473A-BEE4-96E23DAC0F3B}" name="4º" dataDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{850D29A6-7DF0-4D99-8BA8-FDAD97B3836A}" name="5º" dataDxfId="50"/>
+    <tableColumn id="9" xr3:uid="{D9466A68-3B98-471D-BCE1-46483F4DD230}" name="Media" dataDxfId="49">
       <calculatedColumnFormula>AVERAGE(E36:I36)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8F6954B4-A278-48CA-B49D-589E58277D00}" name="Desvio Padrao" dataDxfId="62">
+    <tableColumn id="10" xr3:uid="{8F6954B4-A278-48CA-B49D-589E58277D00}" name="Desvio Padrao" dataDxfId="48">
       <calculatedColumnFormula>STDEV(E36:I36)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{FF159FCA-34A1-4421-84FE-AD47693752C1}" name="Coef" dataDxfId="61">
+    <tableColumn id="11" xr3:uid="{FF159FCA-34A1-4421-84FE-AD47693752C1}" name="Coef" dataDxfId="47">
       <calculatedColumnFormula>Tabela44[[#This Row],[Media]]/Tabela44[[#This Row],[Desvio Padrao]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{7E3C1865-17A5-4961-ABD3-74B22DEB0342}" name="Teorica" dataDxfId="60">
+    <tableColumn id="12" xr3:uid="{7E3C1865-17A5-4961-ABD3-74B22DEB0342}" name="Teorica" dataDxfId="46">
       <calculatedColumnFormula>AVERAGE(H36:L36)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4135,25 +6984,25 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{82AF8115-A559-4862-BDF8-50BB6853F36E}" name="Tabela19" displayName="Tabela19" ref="B48:M52" totalsRowShown="0" headerRowDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{82AF8115-A559-4862-BDF8-50BB6853F36E}" name="Tabela19" displayName="Tabela19" ref="B48:M52" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="B48:M52" xr:uid="{82AF8115-A559-4862-BDF8-50BB6853F36E}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{F74C00EB-FC87-4815-BD28-90719C9D3C61}" name="gridDimX" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{B4331134-F346-495D-8964-98DE3D9CE04D}" name="blockDimY" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{5FA1AEB0-A017-430A-9E1F-62903E2AF513}" name="blockDimX2" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{4F91BE4A-CEC4-4124-A51B-FB15A3511644}" name="Cuda Kernel" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{24600B71-B055-4ADA-BABB-8E2953774353}" name="1º " dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{44BD8EF7-1CED-4C50-A694-D58009DA34C5}" name="2º" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{FCEF5D46-EF2D-4E67-AFAA-F85EB0A89FAE}" name="3º" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{B78108B0-5606-4EE2-99BF-2DE7CEB79687}" name="4º" dataDxfId="51"/>
-    <tableColumn id="9" xr3:uid="{E750F501-52F2-4866-8EE4-83E2D37E9BD3}" name="5º" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{F74C00EB-FC87-4815-BD28-90719C9D3C61}" name="gridDimX" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{B4331134-F346-495D-8964-98DE3D9CE04D}" name="blockDimY" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{5FA1AEB0-A017-430A-9E1F-62903E2AF513}" name="blockDimX2" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{4F91BE4A-CEC4-4124-A51B-FB15A3511644}" name="Cuda Kernel" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{24600B71-B055-4ADA-BABB-8E2953774353}" name="1º " dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{44BD8EF7-1CED-4C50-A694-D58009DA34C5}" name="2º" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{FCEF5D46-EF2D-4E67-AFAA-F85EB0A89FAE}" name="3º" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{B78108B0-5606-4EE2-99BF-2DE7CEB79687}" name="4º" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{E750F501-52F2-4866-8EE4-83E2D37E9BD3}" name="5º" dataDxfId="36"/>
     <tableColumn id="10" xr3:uid="{FB8EBC34-02A1-4B67-A16E-B9AE8BDCEAF1}" name="Media">
       <calculatedColumnFormula>AVERAGE(F49:J49)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{74FE1162-B0E8-47B0-999F-D3F73408310B}" name="Desvio Padrao">
       <calculatedColumnFormula>STDEV(F49:J49)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{7B668557-A3C5-46A3-A1AE-B3D0572CEAC9}" name="Coef" dataDxfId="49">
+    <tableColumn id="12" xr3:uid="{7B668557-A3C5-46A3-A1AE-B3D0572CEAC9}" name="Coef" dataDxfId="35">
       <calculatedColumnFormula>Tabela19[[#This Row],[Media]]/Tabela19[[#This Row],[Desvio Padrao]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4162,25 +7011,25 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0DF4CF99-5D43-4EB7-8109-3E1E5C20E658}" name="Tabela1310" displayName="Tabela1310" ref="B55:M63" totalsRowShown="0" headerRowDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{0DF4CF99-5D43-4EB7-8109-3E1E5C20E658}" name="Tabela1310" displayName="Tabela1310" ref="B55:M63" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="B55:M63" xr:uid="{0DF4CF99-5D43-4EB7-8109-3E1E5C20E658}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{5A8C6BE7-EA27-413A-A98F-747BB16534ED}" name="gridDimX" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{11103D20-3E1F-4C3E-98B9-51996439D6E0}" name="blockDimX" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{70D05024-75FB-41A0-8A93-88C75820EAED}" name="blockDimY" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{2FE14C0B-2A34-44C0-850D-33BD167EFC36}" name="Cuda Kernel" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{CC63588B-8AF7-4A16-90E0-3DE47EF87D59}" name="1º " dataDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{42901B77-0EA7-4EA4-8E0F-3D7183078B80}" name="2º" dataDxfId="42"/>
-    <tableColumn id="7" xr3:uid="{8255EED9-5C96-44CF-B2CA-FECB3C42236A}" name="3º" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{B9AFA4F2-E217-4A7F-8CAF-6DF52C1DCF88}" name="4º" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{142C8679-3303-4339-A319-2FDD6A151AA6}" name="5º" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{5A8C6BE7-EA27-413A-A98F-747BB16534ED}" name="gridDimX" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{11103D20-3E1F-4C3E-98B9-51996439D6E0}" name="blockDimX" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{70D05024-75FB-41A0-8A93-88C75820EAED}" name="blockDimY" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{2FE14C0B-2A34-44C0-850D-33BD167EFC36}" name="Cuda Kernel" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{CC63588B-8AF7-4A16-90E0-3DE47EF87D59}" name="1º " dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{42901B77-0EA7-4EA4-8E0F-3D7183078B80}" name="2º" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{8255EED9-5C96-44CF-B2CA-FECB3C42236A}" name="3º" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{B9AFA4F2-E217-4A7F-8CAF-6DF52C1DCF88}" name="4º" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{142C8679-3303-4339-A319-2FDD6A151AA6}" name="5º" dataDxfId="25"/>
     <tableColumn id="10" xr3:uid="{9C66C7D3-F551-46C7-807A-E96D7B24F0CB}" name="Media">
       <calculatedColumnFormula>AVERAGE(F56:J56)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{5D503643-967F-44FB-92A2-2560EA922640}" name="Desvio Padrao">
       <calculatedColumnFormula>STDEV(F56:J56)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{6FFB1603-AF30-4130-A858-4F07DC4B2CC6}" name="Coef" dataDxfId="38">
+    <tableColumn id="12" xr3:uid="{6FFB1603-AF30-4130-A858-4F07DC4B2CC6}" name="Coef" dataDxfId="24">
       <calculatedColumnFormula>Tabela1310[[#This Row],[Media]]/Tabela1310[[#This Row],[Desvio Padrao]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4189,21 +7038,21 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C4BDEC98-048A-41C3-9600-257826FE637A}" name="Tabela6" displayName="Tabela6" ref="E4:N15" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C4BDEC98-048A-41C3-9600-257826FE637A}" name="Tabela6" displayName="Tabela6" ref="E4:N15" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="E4:N15" xr:uid="{C4BDEC98-048A-41C3-9600-257826FE637A}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8F97CC66-24FB-44F5-A370-383AF407BA62}" name="gridDimX" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{97B78A84-BCA7-4DFA-A177-A048B25373A3}" name="blockDimX2" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{1D9AE1D5-3FEF-491C-844D-5EAC3F5575D9}" name="Cuda Kernel" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{F8DAA291-A4D4-47AC-A138-F08945C6EC17}" name="1º " dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{B082E383-C01D-4440-96F9-08FF57731764}" name="2º" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{5C67B0F9-7FE6-4611-B4CB-E667C16968E8}" name="3º" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{2673E548-A356-4007-86E9-82092FAD0941}" name="4º" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{1DFCE80B-445A-46C6-96D5-22AFD0947C3C}" name="5º" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{36F6B6F2-37F0-4E9C-B997-EBB3FCC21F8E}" name="Media" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{8F97CC66-24FB-44F5-A370-383AF407BA62}" name="gridDimX" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{97B78A84-BCA7-4DFA-A177-A048B25373A3}" name="blockDimX2" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{1D9AE1D5-3FEF-491C-844D-5EAC3F5575D9}" name="Cuda Kernel" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{F8DAA291-A4D4-47AC-A138-F08945C6EC17}" name="1º " dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{B082E383-C01D-4440-96F9-08FF57731764}" name="2º" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{5C67B0F9-7FE6-4611-B4CB-E667C16968E8}" name="3º" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{2673E548-A356-4007-86E9-82092FAD0941}" name="4º" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{1DFCE80B-445A-46C6-96D5-22AFD0947C3C}" name="5º" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{36F6B6F2-37F0-4E9C-B997-EBB3FCC21F8E}" name="Media" dataDxfId="13">
       <calculatedColumnFormula>AVERAGE(H5:L5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{73A090F1-E46D-4C38-A71C-F948FD646066}" name="Desvio Padrao" dataDxfId="26">
+    <tableColumn id="10" xr3:uid="{73A090F1-E46D-4C38-A71C-F948FD646066}" name="Desvio Padrao" dataDxfId="12">
       <calculatedColumnFormula>STDEV(H5:L5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4212,21 +7061,21 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{98392A67-6EED-446B-9173-38FE0E72E529}" name="Tabela7" displayName="Tabela7" ref="E18:N29" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{98392A67-6EED-446B-9173-38FE0E72E529}" name="Tabela7" displayName="Tabela7" ref="E18:N29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="E18:N29" xr:uid="{98392A67-6EED-446B-9173-38FE0E72E529}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1BB353E0-9AF2-4592-9468-44F298D46DD1}" name="gridDimX" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{C638798C-4E4E-4C13-9F16-0A8CFEA63919}" name="blockDimX2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{93376937-EB3C-40D4-AF4B-EDC46A2822C1}" name="Cuda Kernel" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{6E8C9373-2253-4422-857F-BAE20575B3E9}" name="1º " dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{A132DC22-ED28-495A-B0BB-BF6B9CCE3C58}" name="2º" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{08528A78-1570-40A8-B01B-99C3249A48C6}" name="3º" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{B80DD6A3-A55B-40C2-AA99-A35DFC438D20}" name="4º" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{7ACC0343-8EFF-4821-ABA0-727221996F3B}" name="5º" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{F34863BD-7004-4562-9C0C-3D2BF350EDA1}" name="Media" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{1BB353E0-9AF2-4592-9468-44F298D46DD1}" name="gridDimX" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C638798C-4E4E-4C13-9F16-0A8CFEA63919}" name="blockDimX2" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{93376937-EB3C-40D4-AF4B-EDC46A2822C1}" name="Cuda Kernel" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{6E8C9373-2253-4422-857F-BAE20575B3E9}" name="1º " dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{A132DC22-ED28-495A-B0BB-BF6B9CCE3C58}" name="2º" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{08528A78-1570-40A8-B01B-99C3249A48C6}" name="3º" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{B80DD6A3-A55B-40C2-AA99-A35DFC438D20}" name="4º" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{7ACC0343-8EFF-4821-ABA0-727221996F3B}" name="5º" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{F34863BD-7004-4562-9C0C-3D2BF350EDA1}" name="Media" dataDxfId="1">
       <calculatedColumnFormula>AVERAGE(Tabela7[[#This Row],[1º ]:[5º]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{05F5711A-CE65-4A09-B77B-AFA8CFD980EE}" name="Desvio Padrao" dataDxfId="14">
+    <tableColumn id="10" xr3:uid="{05F5711A-CE65-4A09-B77B-AFA8CFD980EE}" name="Desvio Padrao" dataDxfId="0">
       <calculatedColumnFormula>STDEV(Tabela7[[#This Row],[1º ]:[5º]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4499,8 +7348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC25" sqref="AC25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4525,6 +7374,10 @@
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:16" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>2^C4</f>
+        <v>1</v>
+      </c>
       <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
@@ -4544,6 +7397,10 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <f>2^C5</f>
+        <v>2</v>
+      </c>
       <c r="B3" s="23" t="s">
         <v>4</v>
       </c>
@@ -4583,6 +7440,10 @@
       <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>2^C6</f>
+        <v>4</v>
+      </c>
       <c r="B4" s="25">
         <v>10</v>
       </c>
@@ -4624,13 +7485,13 @@
         <v>0.23582</v>
       </c>
       <c r="N4" s="1"/>
-      <c r="O4">
-        <f>2^C4</f>
-        <v>1</v>
-      </c>
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>2^C7</f>
+        <v>8</v>
+      </c>
       <c r="B5" s="3">
         <v>9</v>
       </c>
@@ -4673,13 +7534,13 @@
         <v>0.11791</v>
       </c>
       <c r="N5" s="1"/>
-      <c r="O5">
-        <f t="shared" ref="O5:O14" si="2">2^C5</f>
-        <v>2</v>
-      </c>
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>2^C8</f>
+        <v>16</v>
+      </c>
       <c r="B6" s="25">
         <v>8</v>
       </c>
@@ -4717,17 +7578,17 @@
         <v>15.62628001166753</v>
       </c>
       <c r="M6" s="26">
-        <f t="shared" ref="M6:M9" si="3">M5/2</f>
+        <f t="shared" ref="M6:M9" si="2">M5/2</f>
         <v>5.8955E-2</v>
       </c>
       <c r="N6" s="1"/>
-      <c r="O6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
       <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>2^C9</f>
+        <v>32</v>
+      </c>
       <c r="B7" s="3">
         <v>7</v>
       </c>
@@ -4765,17 +7626,17 @@
         <v>59.723550624918751</v>
       </c>
       <c r="M7" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.94775E-2</v>
       </c>
       <c r="N7" s="1"/>
-      <c r="O7">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
       <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>2^C10</f>
+        <v>64</v>
+      </c>
       <c r="B8" s="25">
         <v>6</v>
       </c>
@@ -4813,17 +7674,17 @@
         <v>140.63392523394177</v>
       </c>
       <c r="M8" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.473875E-2</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>2^C11</f>
+        <v>128</v>
+      </c>
       <c r="B9" s="27">
         <v>5</v>
       </c>
@@ -4861,17 +7722,17 @@
         <v>310.31553022993637</v>
       </c>
       <c r="M9" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>7.3693750000000001E-3</v>
       </c>
       <c r="N9" s="1"/>
-      <c r="O9">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>2^C12</f>
+        <v>256</v>
+      </c>
       <c r="B10" s="25">
         <v>4</v>
       </c>
@@ -4913,13 +7774,13 @@
         <v>7.3693999999999999E-3</v>
       </c>
       <c r="N10" s="1"/>
-      <c r="O10">
-        <f t="shared" si="2"/>
-        <v>64</v>
-      </c>
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>2^C13</f>
+        <v>512</v>
+      </c>
       <c r="B11" s="3">
         <v>3</v>
       </c>
@@ -4957,17 +7818,17 @@
         <v>65.188008387366182</v>
       </c>
       <c r="M11" s="26">
-        <f t="shared" ref="M11:M14" si="4">0.0073694</f>
+        <f t="shared" ref="M11:M14" si="3">0.0073694</f>
         <v>7.3693999999999999E-3</v>
       </c>
       <c r="N11" s="1"/>
-      <c r="O11">
-        <f t="shared" si="2"/>
-        <v>128</v>
-      </c>
       <c r="P11" s="1"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>2^C14</f>
+        <v>1024</v>
+      </c>
       <c r="B12" s="25">
         <v>2</v>
       </c>
@@ -5005,14 +7866,10 @@
         <v>42.534565109646636</v>
       </c>
       <c r="M12" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.3693999999999999E-3</v>
       </c>
       <c r="N12" s="1"/>
-      <c r="O12">
-        <f t="shared" si="2"/>
-        <v>256</v>
-      </c>
       <c r="P12" s="1"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -5053,14 +7910,10 @@
         <v>56.574893584264082</v>
       </c>
       <c r="M13" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.3693999999999999E-3</v>
       </c>
       <c r="N13" s="1"/>
-      <c r="O13">
-        <f t="shared" si="2"/>
-        <v>512</v>
-      </c>
       <c r="P13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -5101,14 +7954,10 @@
         <v>186.55337011910066</v>
       </c>
       <c r="M14" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.3693999999999999E-3</v>
       </c>
       <c r="N14" s="1"/>
-      <c r="O14">
-        <f t="shared" si="2"/>
-        <v>1024</v>
-      </c>
       <c r="P14" s="1"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -5196,11 +8045,11 @@
         <v>0.14230000000000001</v>
       </c>
       <c r="K17" s="38">
-        <f t="shared" ref="K17:K22" si="5">AVERAGE(F17:J17)</f>
+        <f t="shared" ref="K17:K22" si="4">AVERAGE(F17:J17)</f>
         <v>0.14287999999999998</v>
       </c>
       <c r="L17" s="38">
-        <f t="shared" ref="L17:L22" si="6">STDEV(F17:J17)</f>
+        <f t="shared" ref="L17:L22" si="5">STDEV(F17:J17)</f>
         <v>4.6043457732885401E-4</v>
       </c>
       <c r="M17" s="39">
@@ -5239,11 +8088,11 @@
         <v>0.1522</v>
       </c>
       <c r="K18" s="14">
+        <f t="shared" si="4"/>
+        <v>0.15255999999999997</v>
+      </c>
+      <c r="L18" s="14">
         <f t="shared" si="5"/>
-        <v>0.15255999999999997</v>
-      </c>
-      <c r="L18" s="14">
-        <f t="shared" si="6"/>
         <v>1.1436782764396626E-3</v>
       </c>
       <c r="M18" s="31">
@@ -5282,11 +8131,11 @@
         <v>0.1535</v>
       </c>
       <c r="K19" s="13">
+        <f t="shared" si="4"/>
+        <v>0.15336</v>
+      </c>
+      <c r="L19" s="13">
         <f t="shared" si="5"/>
-        <v>0.15336</v>
-      </c>
-      <c r="L19" s="13">
-        <f t="shared" si="6"/>
         <v>2.7018512172212754E-4</v>
       </c>
       <c r="M19" s="30">
@@ -5325,11 +8174,11 @@
         <v>0.15770000000000001</v>
       </c>
       <c r="K20" s="14">
+        <f t="shared" si="4"/>
+        <v>0.15615999999999999</v>
+      </c>
+      <c r="L20" s="14">
         <f t="shared" si="5"/>
-        <v>0.15615999999999999</v>
-      </c>
-      <c r="L20" s="14">
-        <f t="shared" si="6"/>
         <v>9.5289033996573467E-4</v>
       </c>
       <c r="M20" s="31">
@@ -5368,11 +8217,11 @@
         <v>0.20960000000000001</v>
       </c>
       <c r="K21" s="13">
+        <f t="shared" si="4"/>
+        <v>0.20762</v>
+      </c>
+      <c r="L21" s="13">
         <f t="shared" si="5"/>
-        <v>0.20762</v>
-      </c>
-      <c r="L21" s="13">
-        <f t="shared" si="6"/>
         <v>1.4669696656713863E-3</v>
       </c>
       <c r="M21" s="30">
@@ -5411,11 +8260,11 @@
         <v>0.23219999999999999</v>
       </c>
       <c r="K22" s="1">
+        <f t="shared" si="4"/>
+        <v>0.23494000000000001</v>
+      </c>
+      <c r="L22" s="1">
         <f t="shared" si="5"/>
-        <v>0.23494000000000001</v>
-      </c>
-      <c r="L22" s="1">
-        <f t="shared" si="6"/>
         <v>1.816039647144308E-3</v>
       </c>
       <c r="M22" s="6">
@@ -5501,11 +8350,11 @@
         <v>0.14230000000000001</v>
       </c>
       <c r="K25" s="38">
-        <f t="shared" ref="K25" si="7">AVERAGE(F25:J25)</f>
+        <f t="shared" ref="K25" si="6">AVERAGE(F25:J25)</f>
         <v>0.14287999999999998</v>
       </c>
       <c r="L25" s="38">
-        <f t="shared" ref="L25" si="8">STDEV(F25:J25)</f>
+        <f t="shared" ref="L25" si="7">STDEV(F25:J25)</f>
         <v>4.6043457732885401E-4</v>
       </c>
       <c r="M25" s="39" t="e">
@@ -5544,11 +8393,11 @@
         <v>0.14729999999999999</v>
       </c>
       <c r="K26" s="14">
-        <f t="shared" ref="K26:K30" si="9">AVERAGE(F26:J26)</f>
+        <f t="shared" ref="K26:K30" si="8">AVERAGE(F26:J26)</f>
         <v>0.14687999999999998</v>
       </c>
       <c r="L26" s="14">
-        <f t="shared" ref="L26:L30" si="10">STDEV(F26:J26)</f>
+        <f t="shared" ref="L26:L30" si="9">STDEV(F26:J26)</f>
         <v>4.9699094559156631E-4</v>
       </c>
       <c r="M26" s="31" t="e">
@@ -5587,11 +8436,11 @@
         <v>0.15179999999999999</v>
       </c>
       <c r="K27" s="13">
+        <f t="shared" si="8"/>
+        <v>0.15201999999999999</v>
+      </c>
+      <c r="L27" s="13">
         <f t="shared" si="9"/>
-        <v>0.15201999999999999</v>
-      </c>
-      <c r="L27" s="13">
-        <f t="shared" si="10"/>
         <v>5.3572380943916174E-4</v>
       </c>
       <c r="M27" s="30" t="e">
@@ -5629,11 +8478,11 @@
         <v>0.15440000000000001</v>
       </c>
       <c r="K28" s="14">
+        <f t="shared" si="8"/>
+        <v>0.15514</v>
+      </c>
+      <c r="L28" s="14">
         <f t="shared" si="9"/>
-        <v>0.15514</v>
-      </c>
-      <c r="L28" s="14">
-        <f t="shared" si="10"/>
         <v>7.9561297123664461E-4</v>
       </c>
       <c r="M28" s="31" t="e">
@@ -5671,11 +8520,11 @@
         <v>0.16159999999999999</v>
       </c>
       <c r="K29" s="13">
+        <f t="shared" si="8"/>
+        <v>0.16099999999999998</v>
+      </c>
+      <c r="L29" s="13">
         <f t="shared" si="9"/>
-        <v>0.16099999999999998</v>
-      </c>
-      <c r="L29" s="13">
-        <f t="shared" si="10"/>
         <v>5.8736700622353556E-4</v>
       </c>
       <c r="M29" s="30" t="e">
@@ -5713,11 +8562,11 @@
         <v>0.16819999999999999</v>
       </c>
       <c r="K30" s="33">
+        <f t="shared" si="8"/>
+        <v>0.16838000000000003</v>
+      </c>
+      <c r="L30" s="33">
         <f t="shared" si="9"/>
-        <v>0.16838000000000003</v>
-      </c>
-      <c r="L30" s="33">
-        <f t="shared" si="10"/>
         <v>7.190271204898991E-4</v>
       </c>
       <c r="M30" s="11" t="e">
@@ -5806,11 +8655,11 @@
         <v>0.12429999999999999</v>
       </c>
       <c r="J36" s="5">
-        <f t="shared" ref="J36:J46" si="11">AVERAGE(E36:I36)</f>
+        <f t="shared" ref="J36:J46" si="10">AVERAGE(E36:I36)</f>
         <v>0.12426</v>
       </c>
       <c r="K36" s="5">
-        <f t="shared" ref="K36:K46" si="12">STDEV(E36:I36)</f>
+        <f t="shared" ref="K36:K46" si="11">STDEV(E36:I36)</f>
         <v>3.2093613071762674E-4</v>
       </c>
       <c r="L36" s="5">
@@ -5847,11 +8696,11 @@
         <v>9.7530000000000006E-2</v>
       </c>
       <c r="J37" s="5">
+        <f t="shared" si="10"/>
+        <v>9.2901999999999998E-2</v>
+      </c>
+      <c r="K37" s="5">
         <f t="shared" si="11"/>
-        <v>9.2901999999999998E-2</v>
-      </c>
-      <c r="K37" s="5">
-        <f t="shared" si="12"/>
         <v>7.347984077282696E-3</v>
       </c>
       <c r="L37" s="5">
@@ -5889,11 +8738,11 @@
         <v>8.1769999999999995E-2</v>
       </c>
       <c r="J38" s="5">
+        <f t="shared" si="10"/>
+        <v>8.1788E-2</v>
+      </c>
+      <c r="K38" s="5">
         <f t="shared" si="11"/>
-        <v>8.1788E-2</v>
-      </c>
-      <c r="K38" s="5">
-        <f t="shared" si="12"/>
         <v>4.5497252664312712E-5</v>
       </c>
       <c r="L38" s="5">
@@ -5901,7 +8750,7 @@
         <v>1797.6470052696861</v>
       </c>
       <c r="M38" s="26">
-        <f t="shared" ref="M38:M39" si="13">M37/2</f>
+        <f t="shared" ref="M38:M39" si="12">M37/2</f>
         <v>3.1064999999999999E-2</v>
       </c>
     </row>
@@ -5934,11 +8783,11 @@
         <v>8.1570000000000004E-2</v>
       </c>
       <c r="J39" s="19">
+        <f t="shared" si="10"/>
+        <v>8.1566E-2</v>
+      </c>
+      <c r="K39" s="19">
         <f t="shared" si="11"/>
-        <v>8.1566E-2</v>
-      </c>
-      <c r="K39" s="19">
-        <f t="shared" si="12"/>
         <v>3.3615472627945877E-5</v>
       </c>
       <c r="L39" s="19">
@@ -5946,7 +8795,7 @@
         <v>2426.4421596200004</v>
       </c>
       <c r="M39" s="26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.5532499999999999E-2</v>
       </c>
     </row>
@@ -5976,11 +8825,11 @@
         <v>9.2490000000000003E-2</v>
       </c>
       <c r="J40" s="5">
+        <f t="shared" si="10"/>
+        <v>9.2508000000000007E-2</v>
+      </c>
+      <c r="K40" s="5">
         <f t="shared" si="11"/>
-        <v>9.2508000000000007E-2</v>
-      </c>
-      <c r="K40" s="5">
-        <f t="shared" si="12"/>
         <v>2.6832815729994057E-5</v>
       </c>
       <c r="L40" s="5">
@@ -6018,11 +8867,11 @@
         <v>0.1183</v>
       </c>
       <c r="J41" s="5">
+        <f t="shared" si="10"/>
+        <v>0.11826</v>
+      </c>
+      <c r="K41" s="5">
         <f t="shared" si="11"/>
-        <v>0.11826</v>
-      </c>
-      <c r="K41" s="5">
-        <f t="shared" si="12"/>
         <v>5.4772255750518179E-5</v>
       </c>
       <c r="L41" s="5">
@@ -6030,7 +8879,7 @@
         <v>2159.1223216853032</v>
       </c>
       <c r="M41" s="26">
-        <f t="shared" ref="M41:M46" si="14">M40</f>
+        <f t="shared" ref="M41:M46" si="13">M40</f>
         <v>1.5532499999999999E-2</v>
       </c>
     </row>
@@ -6060,11 +8909,11 @@
         <v>0.13289999999999999</v>
       </c>
       <c r="J42" s="5">
+        <f t="shared" si="10"/>
+        <v>0.13302</v>
+      </c>
+      <c r="K42" s="5">
         <f t="shared" si="11"/>
-        <v>0.13302</v>
-      </c>
-      <c r="K42" s="5">
-        <f t="shared" si="12"/>
         <v>8.366600265340829E-5</v>
       </c>
       <c r="L42" s="5">
@@ -6072,7 +8921,7 @@
         <v>1589.8930961365963</v>
       </c>
       <c r="M42" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.5532499999999999E-2</v>
       </c>
       <c r="O42" s="12"/>
@@ -6103,11 +8952,11 @@
         <v>0.1414</v>
       </c>
       <c r="J43" s="5">
+        <f t="shared" si="10"/>
+        <v>0.1414</v>
+      </c>
+      <c r="K43" s="5">
         <f t="shared" si="11"/>
-        <v>0.1414</v>
-      </c>
-      <c r="K43" s="5">
-        <f t="shared" si="12"/>
         <v>7.0710678118646961E-5</v>
       </c>
       <c r="L43" s="5">
@@ -6115,7 +8964,7 @@
         <v>1999.6979771957767</v>
       </c>
       <c r="M43" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.5532499999999999E-2</v>
       </c>
     </row>
@@ -6145,11 +8994,11 @@
         <v>0.24249999999999999</v>
       </c>
       <c r="J44" s="5">
+        <f t="shared" si="10"/>
+        <v>0.24237999999999998</v>
+      </c>
+      <c r="K44" s="5">
         <f t="shared" si="11"/>
-        <v>0.24237999999999998</v>
-      </c>
-      <c r="K44" s="5">
-        <f t="shared" si="12"/>
         <v>1.2357184145265492E-3</v>
       </c>
       <c r="L44" s="5">
@@ -6157,7 +9006,7 @@
         <v>196.14500937324382</v>
       </c>
       <c r="M44" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.5532499999999999E-2</v>
       </c>
     </row>
@@ -6187,11 +9036,11 @@
         <v>0.47689999999999999</v>
       </c>
       <c r="J45" s="5">
+        <f t="shared" si="10"/>
+        <v>0.47531999999999996</v>
+      </c>
+      <c r="K45" s="5">
         <f t="shared" si="11"/>
-        <v>0.47531999999999996</v>
-      </c>
-      <c r="K45" s="5">
-        <f t="shared" si="12"/>
         <v>1.3700364958642577E-3</v>
       </c>
       <c r="L45" s="5">
@@ -6199,7 +9048,7 @@
         <v>346.93966287383802</v>
       </c>
       <c r="M45" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.5532499999999999E-2</v>
       </c>
     </row>
@@ -6229,11 +9078,11 @@
         <v>1.0209999999999999</v>
       </c>
       <c r="J46" s="5">
+        <f t="shared" si="10"/>
+        <v>1.0197999999999998</v>
+      </c>
+      <c r="K46" s="5">
         <f t="shared" si="11"/>
-        <v>1.0197999999999998</v>
-      </c>
-      <c r="K46" s="5">
-        <f t="shared" si="12"/>
         <v>2.167948338867836E-3</v>
       </c>
       <c r="L46" s="5">
@@ -6241,7 +9090,7 @@
         <v>470.39866297393797</v>
       </c>
       <c r="M46" s="26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>1.5532499999999999E-2</v>
       </c>
     </row>
@@ -6330,11 +9179,11 @@
         <v>8.1570000000000004E-2</v>
       </c>
       <c r="K49" s="38">
-        <f t="shared" ref="K49:K52" si="15">AVERAGE(F49:J49)</f>
+        <f t="shared" ref="K49:K52" si="14">AVERAGE(F49:J49)</f>
         <v>8.1566E-2</v>
       </c>
       <c r="L49" s="38">
-        <f t="shared" ref="L49:L52" si="16">STDEV(F49:J49)</f>
+        <f t="shared" ref="L49:L52" si="15">STDEV(F49:J49)</f>
         <v>3.3615472627945877E-5</v>
       </c>
       <c r="M49" s="39">
@@ -6372,11 +9221,11 @@
         <v>0.1522</v>
       </c>
       <c r="K50" s="14">
+        <f t="shared" si="14"/>
+        <v>9.5888000000000001E-2</v>
+      </c>
+      <c r="L50" s="14">
         <f t="shared" si="15"/>
-        <v>9.5888000000000001E-2</v>
-      </c>
-      <c r="L50" s="14">
-        <f t="shared" si="16"/>
         <v>3.1479380076488157E-2</v>
       </c>
       <c r="M50" s="31">
@@ -6414,11 +9263,11 @@
         <v>9.8250000000000004E-2</v>
       </c>
       <c r="K51" s="13">
+        <f t="shared" si="14"/>
+        <v>9.7808000000000006E-2</v>
+      </c>
+      <c r="L51" s="13">
         <f t="shared" si="15"/>
-        <v>9.7808000000000006E-2</v>
-      </c>
-      <c r="L51" s="13">
-        <f t="shared" si="16"/>
         <v>1.0034789484588097E-3</v>
       </c>
       <c r="M51" s="30">
@@ -6456,11 +9305,11 @@
         <v>0.12429999999999999</v>
       </c>
       <c r="K52" s="14">
+        <f t="shared" si="14"/>
+        <v>0.12418</v>
+      </c>
+      <c r="L52" s="14">
         <f t="shared" si="15"/>
-        <v>0.12418</v>
-      </c>
-      <c r="L52" s="14">
-        <f t="shared" si="16"/>
         <v>1.6431676725154947E-4</v>
       </c>
       <c r="M52" s="31">
@@ -6548,11 +9397,11 @@
         <v>8.1570000000000004E-2</v>
       </c>
       <c r="K56" s="38">
-        <f t="shared" ref="K56:K61" si="17">AVERAGE(F56:J56)</f>
+        <f t="shared" ref="K56:K61" si="16">AVERAGE(F56:J56)</f>
         <v>8.1566E-2</v>
       </c>
       <c r="L56" s="38">
-        <f t="shared" ref="L56:L61" si="18">STDEV(F56:J56)</f>
+        <f t="shared" ref="L56:L61" si="17">STDEV(F56:J56)</f>
         <v>3.3615472627945877E-5</v>
       </c>
       <c r="M56" s="39">
@@ -6589,11 +9438,11 @@
         <v>9.2340000000000005E-2</v>
       </c>
       <c r="K57" s="14">
+        <f t="shared" si="16"/>
+        <v>9.2310000000000003E-2</v>
+      </c>
+      <c r="L57" s="14">
         <f t="shared" si="17"/>
-        <v>9.2310000000000003E-2</v>
-      </c>
-      <c r="L57" s="14">
-        <f t="shared" si="18"/>
         <v>2.4494897427833618E-5</v>
       </c>
       <c r="M57" s="31">
@@ -6630,11 +9479,11 @@
         <v>0.1182</v>
       </c>
       <c r="K58" s="13">
+        <f t="shared" si="16"/>
+        <v>0.11838</v>
+      </c>
+      <c r="L58" s="13">
         <f t="shared" si="17"/>
-        <v>0.11838</v>
-      </c>
-      <c r="L58" s="13">
-        <f t="shared" si="18"/>
         <v>1.3038404810405033E-4</v>
       </c>
       <c r="M58" s="30">
@@ -6671,11 +9520,11 @@
         <v>0.13320000000000001</v>
       </c>
       <c r="K59" s="14">
+        <f t="shared" si="16"/>
+        <v>0.13317999999999999</v>
+      </c>
+      <c r="L59" s="14">
         <f t="shared" si="17"/>
-        <v>0.13317999999999999</v>
-      </c>
-      <c r="L59" s="14">
-        <f t="shared" si="18"/>
         <v>8.3666002653411611E-5</v>
       </c>
       <c r="M59" s="31">
@@ -6712,11 +9561,11 @@
         <v>0.1414</v>
       </c>
       <c r="K60" s="34">
+        <f t="shared" si="16"/>
+        <v>0.14138000000000001</v>
+      </c>
+      <c r="L60" s="34">
         <f t="shared" si="17"/>
-        <v>0.14138000000000001</v>
-      </c>
-      <c r="L60" s="34">
-        <f t="shared" si="18"/>
         <v>8.3666002653398329E-5</v>
       </c>
       <c r="M60" s="35">
@@ -6753,11 +9602,11 @@
         <v>0.24049999999999999</v>
       </c>
       <c r="K61" s="5">
+        <f t="shared" si="16"/>
+        <v>0.24030000000000001</v>
+      </c>
+      <c r="L61" s="5">
         <f t="shared" si="17"/>
-        <v>0.24030000000000001</v>
-      </c>
-      <c r="L61" s="5">
-        <f t="shared" si="18"/>
         <v>6.0415229867972868E-4</v>
       </c>
       <c r="M61" s="6">
@@ -6911,11 +9760,11 @@
         <v>0.23580000000000001</v>
       </c>
       <c r="K98" s="5">
-        <f t="shared" ref="K98:K108" si="19">AVERAGE(F98:J98)</f>
+        <f t="shared" ref="K98:K108" si="18">AVERAGE(F98:J98)</f>
         <v>0.23529999999999998</v>
       </c>
       <c r="L98" s="5">
-        <f t="shared" ref="L98:L108" si="20">STDEV(F98:J98)</f>
+        <f t="shared" ref="L98:L108" si="19">STDEV(F98:J98)</f>
         <v>7.6720271115266582E-3</v>
       </c>
     </row>
@@ -6945,11 +9794,11 @@
         <v>0.18429999999999999</v>
       </c>
       <c r="K99" s="5">
+        <f t="shared" si="18"/>
+        <v>0.20311999999999997</v>
+      </c>
+      <c r="L99" s="5">
         <f t="shared" si="19"/>
-        <v>0.20311999999999997</v>
-      </c>
-      <c r="L99" s="5">
-        <f t="shared" si="20"/>
         <v>1.0618474466701897E-2</v>
       </c>
     </row>
@@ -6979,11 +9828,11 @@
         <v>0.15490000000000001</v>
       </c>
       <c r="K100" s="5">
+        <f t="shared" si="18"/>
+        <v>0.15518000000000001</v>
+      </c>
+      <c r="L100" s="5">
         <f t="shared" si="19"/>
-        <v>0.15518000000000001</v>
-      </c>
-      <c r="L100" s="5">
-        <f t="shared" si="20"/>
         <v>1.9537144110642187E-3</v>
       </c>
     </row>
@@ -7013,11 +9862,11 @@
         <v>0.1565</v>
       </c>
       <c r="K101" s="5">
+        <f t="shared" si="18"/>
+        <v>0.14364000000000002</v>
+      </c>
+      <c r="L101" s="5">
         <f t="shared" si="19"/>
-        <v>0.14364000000000002</v>
-      </c>
-      <c r="L101" s="5">
-        <f t="shared" si="20"/>
         <v>1.2154957836208241E-2</v>
       </c>
     </row>
@@ -7047,11 +9896,11 @@
         <v>0.155</v>
       </c>
       <c r="K102" s="5">
+        <f t="shared" si="18"/>
+        <v>0.15342</v>
+      </c>
+      <c r="L102" s="5">
         <f t="shared" si="19"/>
-        <v>0.15342</v>
-      </c>
-      <c r="L102" s="5">
-        <f t="shared" si="20"/>
         <v>3.4054368295418436E-3</v>
       </c>
     </row>
@@ -7081,11 +9930,11 @@
         <v>0.14280000000000001</v>
       </c>
       <c r="K103" s="5">
+        <f t="shared" si="18"/>
+        <v>0.13364000000000001</v>
+      </c>
+      <c r="L103" s="5">
         <f t="shared" si="19"/>
-        <v>0.13364000000000001</v>
-      </c>
-      <c r="L103" s="5">
-        <f t="shared" si="20"/>
         <v>1.2910964332690256E-2</v>
       </c>
     </row>
@@ -7115,11 +9964,11 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="K104" s="5">
+        <f t="shared" si="18"/>
+        <v>0.13189999999999999</v>
+      </c>
+      <c r="L104" s="5">
         <f t="shared" si="19"/>
-        <v>0.13189999999999999</v>
-      </c>
-      <c r="L104" s="5">
-        <f t="shared" si="20"/>
         <v>9.1293482790394224E-3</v>
       </c>
     </row>
@@ -7149,11 +9998,11 @@
         <v>0.15379999999999999</v>
       </c>
       <c r="K105" s="5">
+        <f t="shared" si="18"/>
+        <v>0.14487999999999998</v>
+      </c>
+      <c r="L105" s="5">
         <f t="shared" si="19"/>
-        <v>0.14487999999999998</v>
-      </c>
-      <c r="L105" s="5">
-        <f t="shared" si="20"/>
         <v>1.3319609603888546E-2</v>
       </c>
     </row>
@@ -7183,11 +10032,11 @@
         <v>0.1552</v>
       </c>
       <c r="K106" s="5">
+        <f t="shared" si="18"/>
+        <v>0.15722</v>
+      </c>
+      <c r="L106" s="5">
         <f t="shared" si="19"/>
-        <v>0.15722</v>
-      </c>
-      <c r="L106" s="5">
-        <f t="shared" si="20"/>
         <v>2.4833445189904606E-3</v>
       </c>
     </row>
@@ -7217,11 +10066,11 @@
         <v>0.16619999999999999</v>
       </c>
       <c r="K107" s="5">
+        <f t="shared" si="18"/>
+        <v>0.16006000000000001</v>
+      </c>
+      <c r="L107" s="5">
         <f t="shared" si="19"/>
-        <v>0.16006000000000001</v>
-      </c>
-      <c r="L107" s="5">
-        <f t="shared" si="20"/>
         <v>1.0932886169717486E-2</v>
       </c>
     </row>
@@ -7251,11 +10100,11 @@
         <v>0.16880000000000001</v>
       </c>
       <c r="K108" s="5">
+        <f t="shared" si="18"/>
+        <v>0.17069999999999999</v>
+      </c>
+      <c r="L108" s="5">
         <f t="shared" si="19"/>
-        <v>0.17069999999999999</v>
-      </c>
-      <c r="L108" s="5">
-        <f t="shared" si="20"/>
         <v>2.3738154940938475E-3</v>
       </c>
     </row>

</xml_diff>